<commit_message>
add some notes for define
add some notes for define
</commit_message>
<xml_diff>
--- a/GMW A0607 rev01 validation software design.xlsx
+++ b/GMW A0607 rev01 validation software design.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nexteerautomotive-my.sharepoint.com/personal/jeff_gong_nexteer_com/Documents/ESIB_Code/CIB-GWM-A0607/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nz68pn\Documents\GitHub\A0607\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="740" documentId="13_ncr:1_{613782D3-B00E-427D-A0A1-E0F6B1D1A121}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{12ED8527-D45A-455A-BEAC-509B714EB079}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8A4B4D-B44C-4BAB-9092-203DEC7A9099}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAN Summary" sheetId="21" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">'parameter addr 03.01.01'!$A$2:$J$24</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="12">'Random CAN dumps'!$C$115:$N$120</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -187,7 +187,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2864,15 +2864,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="177" formatCode="0.000000"/>
+    <numFmt numFmtId="178" formatCode="0.0"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2919,21 +2919,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2941,7 +2941,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2949,7 +2949,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2957,14 +2957,14 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2972,7 +2972,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2980,7 +2980,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2988,28 +2988,28 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3017,7 +3017,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3025,7 +3025,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Cambria"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -3033,20 +3033,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3060,14 +3060,14 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3078,7 +3078,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3086,8 +3086,15 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3763,12 +3770,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3789,7 +3796,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3928,8 +3935,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4038,39 +4045,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4079,6 +4063,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4088,54 +4073,76 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="20% - 着色 1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 6" xfId="18" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Note" xfId="38" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="39" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="40" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="标题" xfId="40" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题 1" xfId="30" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="标题 2" xfId="31" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="标题 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="标题 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="差" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="29" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="汇总" xfId="41" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="计算" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="检查单元格" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="解释性文本" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="警告文本" xfId="42" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="链接单元格" xfId="35" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="适中" xfId="36" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="输出" xfId="39" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="输入" xfId="34" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="着色 1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="着色 2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="着色 3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="着色 4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="着色 5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="着色 6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="注释" xfId="38" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4188,6 +4195,59 @@
         <a:xfrm>
           <a:off x="0" y="4714875"/>
           <a:ext cx="12285714" cy="5066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>541020</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图形 3" descr="毫无表情的脸，实心填充 纯色填充">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFCA195F-B7B5-48EA-928D-BE2BB97C8067}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12344400" y="3101340"/>
+          <a:ext cx="403860" cy="403860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5458,7 +5518,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5783,26 +5843,26 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="119" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" style="119" customWidth="1"/>
     <col min="2" max="2" width="16" style="52" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="52" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="52" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="37.7109375" customWidth="1"/>
-    <col min="7" max="7" width="35.28515625" customWidth="1"/>
+    <col min="6" max="6" width="37.6640625" customWidth="1"/>
+    <col min="7" max="7" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1"/>
       <c r="D1" s="100"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A2" s="120"/>
       <c r="B2" s="123" t="s">
         <v>754</v>
@@ -5892,7 +5952,7 @@
       <c r="F7" s="126"/>
       <c r="G7" s="126"/>
     </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A8" s="140" t="s">
         <v>753</v>
       </c>
@@ -5915,7 +5975,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="52" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="52" customFormat="1" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A9" s="141"/>
       <c r="B9" s="133" t="s">
         <v>823</v>
@@ -5936,7 +5996,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="52" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A10" s="141"/>
       <c r="B10" s="133" t="s">
         <v>830</v>
@@ -5957,7 +6017,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A11" s="141"/>
       <c r="B11" s="133" t="s">
         <v>822</v>
@@ -5978,7 +6038,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A12" s="141"/>
       <c r="B12" s="133" t="s">
         <v>828</v>
@@ -5999,7 +6059,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A13" s="141"/>
       <c r="B13" s="133" t="s">
         <v>829</v>
@@ -6086,7 +6146,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A18" s="141"/>
       <c r="B18" s="133" t="s">
         <v>856</v>
@@ -6107,7 +6167,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A19" s="142"/>
       <c r="B19" s="133" t="s">
         <v>857</v>
@@ -6151,24 +6211,24 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" customWidth="1"/>
-    <col min="4" max="4" width="103.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="4.85546875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.88671875" customWidth="1"/>
+    <col min="4" max="4" width="103.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5546875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="4.88671875" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="6" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:118" ht="78.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:118" ht="76.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>19</v>
       </c>
@@ -8418,7 +8478,7 @@
       <c r="K85" s="5"/>
       <c r="L85" s="5"/>
     </row>
-    <row r="86" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="5"/>
       <c r="B86" s="19"/>
       <c r="C86" s="19"/>
@@ -8432,20 +8492,20 @@
       <c r="K86" s="7"/>
       <c r="M86" s="11"/>
     </row>
-    <row r="87" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="22"/>
       <c r="B87" s="87"/>
-      <c r="C87" s="156" t="s">
+      <c r="C87" s="166" t="s">
         <v>38</v>
       </c>
-      <c r="D87" s="157"/>
-      <c r="E87" s="157"/>
-      <c r="F87" s="157"/>
-      <c r="G87" s="157"/>
-      <c r="H87" s="157"/>
-      <c r="I87" s="157"/>
-      <c r="J87" s="157"/>
-      <c r="K87" s="158"/>
+      <c r="D87" s="146"/>
+      <c r="E87" s="146"/>
+      <c r="F87" s="146"/>
+      <c r="G87" s="146"/>
+      <c r="H87" s="146"/>
+      <c r="I87" s="146"/>
+      <c r="J87" s="146"/>
+      <c r="K87" s="147"/>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K88" s="24"/>
@@ -8470,6 +8530,7 @@
   <mergeCells count="1">
     <mergeCell ref="C87:K87"/>
   </mergeCells>
+  <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="56" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -8486,19 +8547,19 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.5703125" style="52" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.5546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="52" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="52" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" style="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" style="52" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" style="52" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.88671875" style="52" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" style="52" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" style="52" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="52"/>
+    <col min="10" max="10" width="4.88671875" style="52" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="52"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -11670,6 +11731,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="65" orientation="landscape" r:id="rId1"/>
 </worksheet>
@@ -11683,50 +11745,50 @@
       <selection activeCell="AJ39" sqref="AJ39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.140625" style="52" customWidth="1"/>
-    <col min="2" max="2" width="3.28515625" style="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="52" customWidth="1"/>
-    <col min="4" max="4" width="3.28515625" style="52" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" style="52" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.28515625" style="52" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.85546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="8" max="25" width="3.28515625" style="52" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="3.28515625" style="52" customWidth="1"/>
-    <col min="27" max="27" width="3.7109375" style="52" customWidth="1"/>
-    <col min="28" max="28" width="3.140625" style="52" customWidth="1"/>
-    <col min="29" max="29" width="3.28515625" style="52" customWidth="1"/>
-    <col min="30" max="35" width="3.140625" style="52" customWidth="1"/>
-    <col min="36" max="42" width="3.28515625" style="52" customWidth="1"/>
-    <col min="43" max="51" width="3.140625" style="52" customWidth="1"/>
-    <col min="52" max="53" width="3.28515625" style="52" customWidth="1"/>
-    <col min="54" max="54" width="3.140625" style="52" customWidth="1"/>
-    <col min="55" max="112" width="3.28515625" style="52" customWidth="1"/>
-    <col min="113" max="113" width="3.42578125" style="52" customWidth="1"/>
-    <col min="114" max="114" width="3.28515625" style="52" customWidth="1"/>
-    <col min="115" max="117" width="3.42578125" style="52" customWidth="1"/>
-    <col min="118" max="118" width="3.28515625" style="52" customWidth="1"/>
-    <col min="119" max="119" width="4.5703125" style="52" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="3.28515625" style="52" customWidth="1"/>
-    <col min="121" max="121" width="4.5703125" style="52" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="3.28515625" style="52" customWidth="1"/>
+    <col min="1" max="1" width="39.109375" style="52" customWidth="1"/>
+    <col min="2" max="2" width="3.33203125" style="52" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" style="52" customWidth="1"/>
+    <col min="4" max="4" width="3.33203125" style="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" style="52" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.33203125" style="52" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.88671875" style="52" bestFit="1" customWidth="1"/>
+    <col min="8" max="25" width="3.33203125" style="52" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.33203125" style="52" customWidth="1"/>
+    <col min="27" max="27" width="3.6640625" style="52" customWidth="1"/>
+    <col min="28" max="28" width="3.109375" style="52" customWidth="1"/>
+    <col min="29" max="29" width="3.33203125" style="52" customWidth="1"/>
+    <col min="30" max="35" width="3.109375" style="52" customWidth="1"/>
+    <col min="36" max="42" width="3.33203125" style="52" customWidth="1"/>
+    <col min="43" max="51" width="3.109375" style="52" customWidth="1"/>
+    <col min="52" max="53" width="3.33203125" style="52" customWidth="1"/>
+    <col min="54" max="54" width="3.109375" style="52" customWidth="1"/>
+    <col min="55" max="112" width="3.33203125" style="52" customWidth="1"/>
+    <col min="113" max="113" width="3.44140625" style="52" customWidth="1"/>
+    <col min="114" max="114" width="3.33203125" style="52" customWidth="1"/>
+    <col min="115" max="117" width="3.44140625" style="52" customWidth="1"/>
+    <col min="118" max="118" width="3.33203125" style="52" customWidth="1"/>
+    <col min="119" max="119" width="4.5546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="3.33203125" style="52" customWidth="1"/>
+    <col min="121" max="121" width="4.5546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="3.33203125" style="52" customWidth="1"/>
     <col min="123" max="125" width="3" style="52" customWidth="1"/>
-    <col min="126" max="128" width="3.28515625" style="52" customWidth="1"/>
-    <col min="129" max="129" width="3.5703125" style="52" customWidth="1"/>
-    <col min="130" max="130" width="3.140625" style="52" customWidth="1"/>
+    <col min="126" max="128" width="3.33203125" style="52" customWidth="1"/>
+    <col min="129" max="129" width="3.5546875" style="52" customWidth="1"/>
+    <col min="130" max="130" width="3.109375" style="52" customWidth="1"/>
     <col min="131" max="131" width="4" style="52" customWidth="1"/>
-    <col min="132" max="132" width="3.28515625" style="52" customWidth="1"/>
-    <col min="133" max="133" width="3.7109375" style="52" customWidth="1"/>
-    <col min="134" max="134" width="3.28515625" style="52" customWidth="1"/>
-    <col min="135" max="137" width="3.42578125" style="52" customWidth="1"/>
-    <col min="138" max="138" width="3.7109375" style="52" customWidth="1"/>
-    <col min="139" max="139" width="3.42578125" style="52" customWidth="1"/>
+    <col min="132" max="132" width="3.33203125" style="52" customWidth="1"/>
+    <col min="133" max="133" width="3.6640625" style="52" customWidth="1"/>
+    <col min="134" max="134" width="3.33203125" style="52" customWidth="1"/>
+    <col min="135" max="137" width="3.44140625" style="52" customWidth="1"/>
+    <col min="138" max="138" width="3.6640625" style="52" customWidth="1"/>
+    <col min="139" max="139" width="3.44140625" style="52" customWidth="1"/>
     <col min="140" max="140" width="4" style="52" customWidth="1"/>
-    <col min="141" max="142" width="3.28515625" style="52" customWidth="1"/>
+    <col min="141" max="142" width="3.33203125" style="52" customWidth="1"/>
     <col min="143" max="143" width="3" style="52" customWidth="1"/>
-    <col min="144" max="144" width="3.42578125" style="52" customWidth="1"/>
-    <col min="145" max="16384" width="9.140625" style="52"/>
+    <col min="144" max="144" width="3.44140625" style="52" customWidth="1"/>
+    <col min="145" max="16384" width="9.109375" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:142" x14ac:dyDescent="0.25">
@@ -12274,7 +12336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="52" t="s">
         <v>519</v>
       </c>
@@ -12288,7 +12350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="51">
         <v>1</v>
       </c>
@@ -12299,7 +12361,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="52" t="s">
         <v>520</v>
       </c>
@@ -12313,7 +12375,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="51">
         <v>2</v>
       </c>
@@ -12324,7 +12386,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="52" t="s">
         <v>521</v>
       </c>
@@ -12338,7 +12400,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="51">
         <v>3</v>
       </c>
@@ -12349,7 +12411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="52" t="s">
         <v>522</v>
       </c>
@@ -12363,7 +12425,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="51">
         <v>4</v>
       </c>
@@ -12374,7 +12436,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="52" t="s">
         <v>523</v>
       </c>
@@ -12388,7 +12450,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="51">
         <v>5</v>
       </c>
@@ -12413,7 +12475,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="51">
         <v>6</v>
       </c>
@@ -12424,7 +12486,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="52" t="s">
         <v>553</v>
       </c>
@@ -12438,7 +12500,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="51">
         <v>7</v>
       </c>
@@ -12449,7 +12511,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="52" t="s">
         <v>554</v>
       </c>
@@ -12463,7 +12525,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="51">
         <v>8</v>
       </c>
@@ -12474,7 +12536,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="52" t="s">
         <v>555</v>
       </c>
@@ -12488,7 +12550,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="51">
         <v>9</v>
       </c>
@@ -12512,7 +12574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="52" t="s">
         <v>557</v>
       </c>
@@ -12523,7 +12585,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="51">
         <v>11</v>
       </c>
@@ -12531,7 +12593,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="52" t="s">
         <v>558</v>
       </c>
@@ -12542,7 +12604,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="51">
         <v>12</v>
       </c>
@@ -12550,7 +12612,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="52" t="s">
         <v>559</v>
       </c>
@@ -12561,7 +12623,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="51">
         <v>13</v>
       </c>
@@ -12569,7 +12631,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="52" t="s">
         <v>560</v>
       </c>
@@ -12580,7 +12642,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="51">
         <v>14</v>
       </c>
@@ -12588,7 +12650,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="52" t="s">
         <v>575</v>
       </c>
@@ -12599,7 +12661,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="51">
         <v>15</v>
       </c>
@@ -12607,7 +12669,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="52" t="s">
         <v>561</v>
       </c>
@@ -12618,7 +12680,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="51">
         <v>16</v>
       </c>
@@ -12626,7 +12688,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="52" t="s">
         <v>562</v>
       </c>
@@ -12637,7 +12699,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="51">
         <v>17</v>
       </c>
@@ -12645,7 +12707,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="52" t="s">
         <v>569</v>
       </c>
@@ -12656,7 +12718,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="51">
         <v>18</v>
       </c>
@@ -12672,7 +12734,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="71" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="51">
         <v>19</v>
       </c>
@@ -12680,7 +12742,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="72" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="52" t="s">
         <v>571</v>
       </c>
@@ -12691,7 +12753,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="51">
         <v>20</v>
       </c>
@@ -12699,7 +12761,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="52" t="s">
         <v>572</v>
       </c>
@@ -12710,7 +12772,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="75" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="51">
         <v>21</v>
       </c>
@@ -12718,7 +12780,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="76" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="52" t="s">
         <v>573</v>
       </c>
@@ -12729,7 +12791,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="77" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="51">
         <v>22</v>
       </c>
@@ -12737,7 +12799,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="78" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="52" t="s">
         <v>574</v>
       </c>
@@ -12748,7 +12810,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="51">
         <v>23</v>
       </c>
@@ -12756,7 +12818,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="80" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="52" t="s">
         <v>63</v>
       </c>
@@ -12767,7 +12829,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="51">
         <v>24</v>
       </c>
@@ -12775,7 +12837,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="82" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="52" t="s">
         <v>63</v>
       </c>
@@ -12786,7 +12848,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="83" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="51">
         <v>25</v>
       </c>
@@ -12794,7 +12856,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="84" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="52" t="s">
         <v>63</v>
       </c>
@@ -12805,7 +12867,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="85" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="51">
         <v>26</v>
       </c>
@@ -13129,6 +13191,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToWidth="0" fitToHeight="3" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -13145,10 +13208,10 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="41" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -15216,6 +15279,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="85" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -15233,9 +15297,9 @@
       <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
@@ -16437,6 +16501,7 @@
       <c r="H92" s="52"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="17" scale="54" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -16451,12 +16516,12 @@
       <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="52" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" style="52" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17140,25 +17205,25 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="52" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="52" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="52" customWidth="1"/>
-    <col min="5" max="5" width="49.140625" style="52" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" style="52" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="52"/>
-    <col min="10" max="11" width="13.140625" style="52" customWidth="1"/>
-    <col min="12" max="12" width="57.7109375" style="52" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" style="52" customWidth="1"/>
-    <col min="14" max="14" width="46.5703125" style="52" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="52"/>
-    <col min="16" max="16" width="37.7109375" style="52" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="52"/>
+    <col min="1" max="1" width="3.5546875" style="52" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" style="52" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" style="52" customWidth="1"/>
+    <col min="5" max="5" width="49.109375" style="52" customWidth="1"/>
+    <col min="6" max="6" width="25.5546875" style="52" customWidth="1"/>
+    <col min="7" max="9" width="9.109375" style="52"/>
+    <col min="10" max="11" width="13.109375" style="52" customWidth="1"/>
+    <col min="12" max="12" width="57.6640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" style="52" customWidth="1"/>
+    <col min="14" max="14" width="46.5546875" style="52" customWidth="1"/>
+    <col min="15" max="15" width="9.109375" style="52"/>
+    <col min="16" max="16" width="37.6640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="C1" s="42" t="s">
         <v>80</v>
       </c>
@@ -17194,7 +17259,7 @@
       <c r="F3" s="45"/>
       <c r="G3" s="45"/>
     </row>
-    <row r="4" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B4" s="114"/>
       <c r="C4" s="133" t="s">
         <v>894</v>
@@ -17212,7 +17277,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B5" s="114"/>
       <c r="C5" s="133" t="s">
         <v>895</v>
@@ -17266,7 +17331,7 @@
       <c r="H7" s="101"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B8" s="114"/>
       <c r="C8" s="133" t="s">
         <v>898</v>
@@ -17284,7 +17349,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B9" s="114"/>
       <c r="C9" s="133" t="s">
         <v>899</v>
@@ -17320,7 +17385,7 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B11" s="114"/>
       <c r="C11" s="118" t="s">
         <v>904</v>
@@ -17338,7 +17403,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B12" s="114"/>
       <c r="C12" s="138" t="s">
         <v>901</v>
@@ -17374,7 +17439,7 @@
       <c r="H13" s="101"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B14" s="113"/>
       <c r="C14" s="133" t="s">
         <v>903</v>
@@ -17400,6 +17465,7 @@
     <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="59" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -17414,10 +17480,10 @@
       <selection activeCell="O39" sqref="O39:O41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:4" x14ac:dyDescent="0.25">
@@ -17827,6 +17893,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -17844,22 +17911,22 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" customWidth="1"/>
+    <col min="6" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" customWidth="1"/>
     <col min="10" max="10" width="8" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" customWidth="1"/>
-    <col min="12" max="13" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" customWidth="1"/>
+    <col min="12" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" customWidth="1"/>
     <col min="16" max="16" width="45" customWidth="1"/>
-    <col min="17" max="18" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.4">
-      <c r="B2" s="145" t="s">
+    <row r="2" spans="2:16" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.5">
+      <c r="B2" s="168" t="s">
         <v>736</v>
       </c>
       <c r="C2" s="143"/>
@@ -17874,19 +17941,19 @@
       <c r="L2" s="143"/>
       <c r="M2" s="143"/>
     </row>
-    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="146" t="s">
+    <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="151" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="147"/>
-      <c r="D4" s="147"/>
-      <c r="E4" s="147"/>
-      <c r="F4" s="147"/>
-      <c r="G4" s="147"/>
-      <c r="H4" s="148"/>
-    </row>
-    <row r="6" spans="2:16" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="C4" s="169"/>
+      <c r="D4" s="169"/>
+      <c r="E4" s="169"/>
+      <c r="F4" s="169"/>
+      <c r="G4" s="169"/>
+      <c r="H4" s="170"/>
+    </row>
+    <row r="6" spans="2:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="C6" s="25" t="s">
         <v>60</v>
       </c>
@@ -17897,12 +17964,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="35"/>
       <c r="D7" s="36"/>
       <c r="E7" s="37"/>
     </row>
-    <row r="8" spans="2:16" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="60" t="s">
         <v>99</v>
       </c>
@@ -17937,11 +18004,11 @@
     </row>
     <row r="10" spans="2:16" s="52" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="C10" s="149" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="149"/>
-      <c r="E10" s="149"/>
+      <c r="C10" s="163" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="163"/>
+      <c r="E10" s="163"/>
       <c r="F10" s="28" t="s">
         <v>8</v>
       </c>
@@ -17969,11 +18036,11 @@
     </row>
     <row r="11" spans="2:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
-      <c r="C11" s="149" t="s">
+      <c r="C11" s="163" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="149"/>
-      <c r="E11" s="149"/>
+      <c r="D11" s="163"/>
+      <c r="E11" s="163"/>
       <c r="F11" s="39" t="s">
         <v>11</v>
       </c>
@@ -18003,11 +18070,11 @@
     </row>
     <row r="12" spans="2:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
-      <c r="C12" s="149" t="s">
+      <c r="C12" s="163" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="149"/>
-      <c r="E12" s="149"/>
+      <c r="D12" s="163"/>
+      <c r="E12" s="163"/>
       <c r="F12" s="39" t="s">
         <v>11</v>
       </c>
@@ -18037,11 +18104,11 @@
     </row>
     <row r="13" spans="2:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
-      <c r="C13" s="144" t="s">
+      <c r="C13" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="144"/>
-      <c r="E13" s="144"/>
+      <c r="D13" s="167"/>
+      <c r="E13" s="167"/>
       <c r="F13" s="39" t="s">
         <v>11</v>
       </c>
@@ -18069,11 +18136,11 @@
     </row>
     <row r="14" spans="2:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
-      <c r="C14" s="144" t="s">
+      <c r="C14" s="167" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="144"/>
-      <c r="E14" s="144"/>
+      <c r="D14" s="167"/>
+      <c r="E14" s="167"/>
       <c r="F14" s="39" t="s">
         <v>11</v>
       </c>
@@ -18101,11 +18168,11 @@
     </row>
     <row r="15" spans="2:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
-      <c r="C15" s="144" t="s">
+      <c r="C15" s="167" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="144"/>
-      <c r="E15" s="144"/>
+      <c r="D15" s="167"/>
+      <c r="E15" s="167"/>
       <c r="F15" s="39" t="s">
         <v>11</v>
       </c>
@@ -18133,11 +18200,11 @@
     </row>
     <row r="16" spans="2:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
-      <c r="C16" s="144" t="s">
+      <c r="C16" s="167" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
+      <c r="D16" s="167"/>
+      <c r="E16" s="167"/>
       <c r="F16" s="39" t="s">
         <v>11</v>
       </c>
@@ -18163,12 +18230,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:19" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:19" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
       <c r="E17" s="37"/>
     </row>
-    <row r="18" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="60" t="s">
         <v>99</v>
       </c>
@@ -18211,11 +18278,11 @@
     </row>
     <row r="20" spans="2:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="C20" s="149" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="149"/>
-      <c r="E20" s="149"/>
+      <c r="C20" s="163" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="163"/>
+      <c r="E20" s="163"/>
       <c r="F20" s="28" t="s">
         <v>8</v>
       </c>
@@ -18244,11 +18311,11 @@
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
-      <c r="C21" s="149" t="s">
+      <c r="C21" s="163" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="149"/>
-      <c r="E21" s="149"/>
+      <c r="D21" s="163"/>
+      <c r="E21" s="163"/>
       <c r="F21" s="39" t="s">
         <v>11</v>
       </c>
@@ -18277,11 +18344,11 @@
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
-      <c r="C22" s="149" t="s">
+      <c r="C22" s="163" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="149"/>
-      <c r="E22" s="149"/>
+      <c r="D22" s="163"/>
+      <c r="E22" s="163"/>
       <c r="F22" s="39" t="s">
         <v>11</v>
       </c>
@@ -18310,11 +18377,11 @@
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
-      <c r="C23" s="144" t="s">
+      <c r="C23" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="144"/>
-      <c r="E23" s="144"/>
+      <c r="D23" s="167"/>
+      <c r="E23" s="167"/>
       <c r="F23" s="39" t="s">
         <v>11</v>
       </c>
@@ -18343,11 +18410,11 @@
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="144" t="s">
+      <c r="C24" s="167" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="144"/>
-      <c r="E24" s="144"/>
+      <c r="D24" s="167"/>
+      <c r="E24" s="167"/>
       <c r="F24" s="39" t="s">
         <v>11</v>
       </c>
@@ -18376,11 +18443,11 @@
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
-      <c r="C25" s="144" t="s">
+      <c r="C25" s="167" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="144"/>
-      <c r="E25" s="144"/>
+      <c r="D25" s="167"/>
+      <c r="E25" s="167"/>
       <c r="F25" s="39" t="s">
         <v>11</v>
       </c>
@@ -18409,11 +18476,11 @@
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
-      <c r="C26" s="144" t="s">
+      <c r="C26" s="167" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="144"/>
-      <c r="E26" s="144"/>
+      <c r="D26" s="167"/>
+      <c r="E26" s="167"/>
       <c r="F26" s="39" t="s">
         <v>11</v>
       </c>
@@ -18440,10 +18507,10 @@
       </c>
       <c r="O26" s="52"/>
     </row>
-    <row r="27" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O27" s="52"/>
     </row>
-    <row r="28" spans="2:19" ht="37.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:19" ht="37.799999999999997" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="60" t="s">
         <v>99</v>
       </c>
@@ -18595,7 +18662,7 @@
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="O33" s="52"/>
     </row>
-    <row r="34" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="52"/>
       <c r="C34" s="52"/>
       <c r="D34" s="52"/>
@@ -18611,17 +18678,17 @@
       <c r="N34" s="52"/>
       <c r="O34" s="52"/>
     </row>
-    <row r="35" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="C35" s="162" t="s">
+      <c r="C35" s="144" t="s">
         <v>441</v>
       </c>
-      <c r="D35" s="160"/>
-      <c r="E35" s="160"/>
-      <c r="F35" s="157"/>
-      <c r="G35" s="158"/>
+      <c r="D35" s="145"/>
+      <c r="E35" s="145"/>
+      <c r="F35" s="146"/>
+      <c r="G35" s="147"/>
       <c r="H35" s="52"/>
       <c r="I35" s="52"/>
       <c r="J35" s="52"/>
@@ -18659,12 +18726,12 @@
       <c r="R36" s="52"/>
       <c r="S36" s="52"/>
     </row>
-    <row r="37" spans="1:19" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="37.200000000000003" x14ac:dyDescent="0.25">
       <c r="B37" s="52"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="170"/>
-      <c r="E37" s="149"/>
-      <c r="F37" s="149"/>
+      <c r="D37" s="162"/>
+      <c r="E37" s="163"/>
+      <c r="F37" s="163"/>
       <c r="G37" s="28" t="s">
         <v>1</v>
       </c>
@@ -18694,9 +18761,9 @@
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B38" s="52"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="149"/>
-      <c r="E38" s="149"/>
-      <c r="F38" s="149"/>
+      <c r="D38" s="163"/>
+      <c r="E38" s="163"/>
+      <c r="F38" s="163"/>
       <c r="G38" s="72" t="s">
         <v>11</v>
       </c>
@@ -18725,9 +18792,9 @@
     </row>
     <row r="39" spans="1:19" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="5"/>
-      <c r="D39" s="149"/>
-      <c r="E39" s="149"/>
-      <c r="F39" s="149"/>
+      <c r="D39" s="163"/>
+      <c r="E39" s="163"/>
+      <c r="F39" s="163"/>
       <c r="G39" s="69"/>
       <c r="H39" s="69"/>
       <c r="I39" s="69"/>
@@ -18737,7 +18804,7 @@
       <c r="M39" s="69"/>
       <c r="N39" s="69"/>
     </row>
-    <row r="40" spans="1:19" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="73"/>
       <c r="D40" s="74"/>
       <c r="E40" s="75"/>
@@ -18751,15 +18818,15 @@
       <c r="M40" s="76"/>
       <c r="N40" s="76"/>
     </row>
-    <row r="41" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="C41" s="162" t="s">
+      <c r="C41" s="144" t="s">
         <v>443</v>
       </c>
-      <c r="D41" s="165"/>
-      <c r="E41" s="166"/>
+      <c r="D41" s="154"/>
+      <c r="E41" s="155"/>
       <c r="F41" s="32"/>
       <c r="G41" s="56"/>
       <c r="H41" s="56"/>
@@ -18802,11 +18869,11 @@
       <c r="A43" s="71"/>
       <c r="B43" s="52"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="154" t="s">
+      <c r="D43" s="156" t="s">
         <v>103</v>
       </c>
-      <c r="E43" s="154"/>
-      <c r="F43" s="154"/>
+      <c r="E43" s="156"/>
+      <c r="F43" s="156"/>
       <c r="G43" s="55" t="s">
         <v>11</v>
       </c>
@@ -18836,11 +18903,11 @@
     <row r="44" spans="1:19" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="52"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="154" t="s">
+      <c r="D44" s="156" t="s">
         <v>104</v>
       </c>
-      <c r="E44" s="154"/>
-      <c r="F44" s="154"/>
+      <c r="E44" s="156"/>
+      <c r="F44" s="156"/>
       <c r="G44" s="55" t="s">
         <v>11</v>
       </c>
@@ -18870,11 +18937,11 @@
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B45" s="52"/>
       <c r="C45" s="5"/>
-      <c r="D45" s="167" t="s">
+      <c r="D45" s="157" t="s">
         <v>107</v>
       </c>
-      <c r="E45" s="168"/>
-      <c r="F45" s="169"/>
+      <c r="E45" s="158"/>
+      <c r="F45" s="159"/>
       <c r="G45" s="55"/>
       <c r="H45" s="55" t="s">
         <v>108</v>
@@ -18980,7 +19047,7 @@
       </c>
       <c r="O47" s="52"/>
     </row>
-    <row r="48" spans="1:19" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="73"/>
       <c r="D48" s="74"/>
       <c r="E48" s="75"/>
@@ -18994,15 +19061,15 @@
       <c r="M48" s="76"/>
       <c r="N48" s="76"/>
     </row>
-    <row r="49" spans="2:20" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:20" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="162" t="s">
+      <c r="C49" s="144" t="s">
         <v>442</v>
       </c>
-      <c r="D49" s="165"/>
-      <c r="E49" s="166"/>
+      <c r="D49" s="154"/>
+      <c r="E49" s="155"/>
       <c r="F49" s="32"/>
       <c r="G49" s="56"/>
       <c r="H49" s="56"/>
@@ -19043,7 +19110,7 @@
       <c r="R50" s="52"/>
       <c r="S50" s="52"/>
     </row>
-    <row r="51" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="52"/>
       <c r="C51" s="52"/>
       <c r="D51" s="52"/>
@@ -19059,16 +19126,16 @@
       <c r="N51" s="52"/>
       <c r="O51" s="52"/>
     </row>
-    <row r="52" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="146" t="s">
+    <row r="52" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="151" t="s">
         <v>64</v>
       </c>
-      <c r="C52" s="163"/>
-      <c r="D52" s="163"/>
-      <c r="E52" s="163"/>
-      <c r="F52" s="163"/>
-      <c r="G52" s="163"/>
-      <c r="H52" s="164"/>
+      <c r="C52" s="152"/>
+      <c r="D52" s="152"/>
+      <c r="E52" s="152"/>
+      <c r="F52" s="152"/>
+      <c r="G52" s="152"/>
+      <c r="H52" s="153"/>
       <c r="I52" s="52"/>
       <c r="J52" s="52"/>
       <c r="K52" s="52"/>
@@ -19077,14 +19144,14 @@
       <c r="N52" s="52"/>
       <c r="O52" s="52"/>
     </row>
-    <row r="53" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="159" t="s">
+      <c r="C53" s="160" t="s">
         <v>444</v>
       </c>
-      <c r="D53" s="160"/>
+      <c r="D53" s="145"/>
       <c r="E53" s="161"/>
       <c r="F53" s="77"/>
       <c r="G53" s="77"/>
@@ -19128,11 +19195,11 @@
     <row r="55" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B55" s="52"/>
       <c r="C55" s="78"/>
-      <c r="D55" s="150" t="s">
+      <c r="D55" s="148" t="s">
         <v>118</v>
       </c>
-      <c r="E55" s="151"/>
-      <c r="F55" s="152"/>
+      <c r="E55" s="149"/>
+      <c r="F55" s="150"/>
       <c r="G55" s="81" t="s">
         <v>11</v>
       </c>
@@ -19162,11 +19229,11 @@
     <row r="56" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B56" s="52"/>
       <c r="C56" s="78"/>
-      <c r="D56" s="150" t="s">
+      <c r="D56" s="148" t="s">
         <v>123</v>
       </c>
-      <c r="E56" s="151"/>
-      <c r="F56" s="152"/>
+      <c r="E56" s="149"/>
+      <c r="F56" s="150"/>
       <c r="G56" s="81" t="s">
         <v>124</v>
       </c>
@@ -19271,7 +19338,7 @@
       <c r="M60" s="5"/>
       <c r="O60" s="52"/>
     </row>
-    <row r="61" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="19"/>
       <c r="C61" s="19"/>
       <c r="D61" s="19"/>
@@ -19286,14 +19353,14 @@
       <c r="M61" s="5"/>
       <c r="O61" s="52"/>
     </row>
-    <row r="62" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="C62" s="159" t="s">
+      <c r="C62" s="160" t="s">
         <v>445</v>
       </c>
-      <c r="D62" s="160"/>
+      <c r="D62" s="145"/>
       <c r="E62" s="161"/>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
@@ -19332,11 +19399,11 @@
     </row>
     <row r="64" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
-      <c r="C64" s="154" t="s">
+      <c r="C64" s="156" t="s">
         <v>747</v>
       </c>
-      <c r="D64" s="154"/>
-      <c r="E64" s="154"/>
+      <c r="D64" s="156"/>
+      <c r="E64" s="156"/>
       <c r="F64" s="5" t="s">
         <v>10</v>
       </c>
@@ -19367,9 +19434,9 @@
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B65" s="5"/>
-      <c r="C65" s="155"/>
-      <c r="D65" s="154"/>
-      <c r="E65" s="154"/>
+      <c r="C65" s="165"/>
+      <c r="D65" s="156"/>
+      <c r="E65" s="156"/>
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
       <c r="H65" s="31"/>
@@ -19380,20 +19447,20 @@
       <c r="M65" s="5"/>
       <c r="O65" s="52"/>
     </row>
-    <row r="66" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="156" t="s">
+    <row r="66" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="166" t="s">
         <v>76</v>
       </c>
-      <c r="C67" s="157"/>
-      <c r="D67" s="158"/>
-    </row>
-    <row r="68" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="156" t="s">
+      <c r="C67" s="146"/>
+      <c r="D67" s="147"/>
+    </row>
+    <row r="68" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="166" t="s">
         <v>67</v>
       </c>
-      <c r="C68" s="157"/>
-      <c r="D68" s="158"/>
+      <c r="C68" s="146"/>
+      <c r="D68" s="147"/>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B69" s="41"/>
@@ -19401,31 +19468,12 @@
       <c r="D69" s="41"/>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="153"/>
-      <c r="C70" s="153"/>
-      <c r="D70" s="153"/>
+      <c r="B70" s="164"/>
+      <c r="C70" s="164"/>
+      <c r="D70" s="164"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="B52:H52"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="C62:E62"/>
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B4:H4"/>
@@ -19442,7 +19490,27 @@
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C16:E16"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="B52:H52"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
   </mergeCells>
+  <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="40" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -19457,11 +19525,11 @@
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -19584,6 +19652,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -19597,9 +19666,9 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="72.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="72.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -20561,6 +20630,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -20571,10 +20641,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="55.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="58" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -21055,6 +21125,7 @@
       <c r="P22" s="52"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -21067,25 +21138,25 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="26" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="2" bestFit="1" customWidth="1"/>
@@ -21093,29 +21164,29 @@
     <col min="24" max="24" width="2" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="26" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="32.5703125" customWidth="1"/>
+    <col min="31" max="31" width="32.5546875" customWidth="1"/>
     <col min="32" max="32" width="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="30.5546875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="31.5703125" customWidth="1"/>
+    <col min="35" max="35" width="31.5546875" customWidth="1"/>
     <col min="36" max="36" width="3" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="3" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="33.44140625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="3" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="30" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="3" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="3" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="31.85546875" customWidth="1"/>
+    <col min="45" max="45" width="31.88671875" customWidth="1"/>
     <col min="46" max="46" width="3" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="3" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="3" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="30" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="3" bestFit="1" customWidth="1"/>
@@ -21123,73 +21194,73 @@
     <col min="54" max="54" width="3" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="30" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="3" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="32.44140625" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="3" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="32.44140625" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="3" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="32.44140625" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="3" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="3" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="3" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="3" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="3" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="3" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="3" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="76" max="76" width="3" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="3" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="3" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="82" max="82" width="3" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="3" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="86" max="86" width="3" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="88" max="88" width="3" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="3" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="3" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="3" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="3" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="3" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="100" max="100" width="3" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="3" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="104" max="104" width="3" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="106" max="106" width="3" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="108" max="108" width="3" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="110" max="110" width="3" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="112" max="112" width="3" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="114" max="114" width="3" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="116" max="116" width="3" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="118" max="118" width="3" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="120" max="120" width="3" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="122" max="122" width="3" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:123" s="105" customFormat="1" x14ac:dyDescent="0.25">
@@ -30538,6 +30609,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>